<commit_message>
Add PoC_v2 files and project contents (API keys removed)
</commit_message>
<xml_diff>
--- a/데이터/merged_output_SKT.xlsx
+++ b/데이터/merged_output_SKT.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/c99f2327ed8f6ce6/Desktop/PoC_v2/데이터/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="1" documentId="11_2459FD949144640E62355476585DCE3A87631701" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{0FCDEA52-70B3-4288-83B6-DFDFEF512613}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="11_2459FD949144640E62355476585DCE3A87631701" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D5EF836E-5AF8-4D32-B6F3-D72A56A4287A}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -14221,11 +14221,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E1203"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A863" workbookViewId="0">
+      <selection activeCell="A1203" sqref="A1203"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="3" max="3" width="114.875" customWidth="1"/>
+    <col min="4" max="4" width="19.5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.3">

</xml_diff>